<commit_message>
Agregar Productos, Eliminar productos, nuevo catalogo
</commit_message>
<xml_diff>
--- a/public/database/Trabajos.xlsx
+++ b/public/database/Trabajos.xlsx
@@ -1,86 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ignacio Aguilera\Desktop\Trabajo (SPA)\IvelPink\public\database\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E33C899-7B03-4750-94D6-F694F087E255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
-  <si>
-    <t>NombreCliente</t>
-  </si>
-  <si>
-    <t>EmailCliente</t>
-  </si>
-  <si>
-    <t>TelefonoCliente</t>
-  </si>
-  <si>
-    <t>Estado</t>
-  </si>
-  <si>
-    <t>FechaCreacion</t>
-  </si>
-  <si>
-    <t>2025-08-22T20:07:38.324Z</t>
-  </si>
-  <si>
-    <t>Maivelyn Sanchez</t>
-  </si>
-  <si>
-    <t>ivelpink.cl@gmail.com</t>
-  </si>
-  <si>
-    <t>Ignacio Aguilera</t>
-  </si>
-  <si>
-    <t>plataformas.web.cl@gmail.com</t>
-  </si>
-  <si>
-    <t>Trabajo</t>
-  </si>
-  <si>
-    <t>StockActual</t>
-  </si>
-  <si>
-    <t>StockSolicitado</t>
-  </si>
-  <si>
-    <t>Accesorios</t>
-  </si>
-  <si>
-    <t>Ropa Invierno</t>
-  </si>
-  <si>
-    <t>Carteras</t>
-  </si>
-  <si>
-    <t>TipoTrabajo</t>
-  </si>
-  <si>
-    <t>Pantalones (18 Septiembre)</t>
-  </si>
-</sst>
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -110,28 +65,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -169,7 +116,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -241,7 +188,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -273,20 +220,16 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -408,180 +351,176 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="24.296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.296875" customWidth="1"/>
-    <col min="6" max="6" width="13.59765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.796875" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Trabajo</v>
+      </c>
+      <c r="B1" t="str">
+        <v>TipoTrabajo</v>
+      </c>
+      <c r="C1" t="str">
+        <v>StockActual</v>
+      </c>
+      <c r="D1" t="str">
+        <v>StockSolicitado</v>
+      </c>
+      <c r="E1" t="str">
+        <v>NombreCliente</v>
+      </c>
+      <c r="F1" t="str">
+        <v>EmailCliente</v>
+      </c>
+      <c r="G1" t="str">
+        <v>TelefonoCliente</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Estado</v>
+      </c>
+      <c r="I1" t="str">
+        <v>FechaCreacion</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Arreglos - Ruedos</v>
+      </c>
+      <c r="B2">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" t="s">
-        <v>4</v>
+      <c r="C2" t="str">
+        <v>90</v>
+      </c>
+      <c r="D2" t="str">
+        <v>100</v>
+      </c>
+      <c r="E2" t="str">
+        <v>Maivelyn</v>
+      </c>
+      <c r="F2" t="str">
+        <v>maivelynn@gmail.com</v>
+      </c>
+      <c r="G2" t="str">
+        <v>92929292</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" t="str">
+        <v>2026-01-11T14:32:55.368Z</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2">
-        <v>56936300432</v>
-      </c>
-      <c r="E2">
-        <v>20</v>
-      </c>
-      <c r="F2">
-        <v>20</v>
-      </c>
-      <c r="G2">
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Confección - Vestidos</v>
+      </c>
+      <c r="B3">
         <v>1</v>
       </c>
-      <c r="H2">
-        <v>2</v>
-      </c>
-      <c r="I2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3">
-        <v>56936300432</v>
-      </c>
-      <c r="E3">
-        <v>8</v>
-      </c>
-      <c r="F3">
-        <v>30</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
+      <c r="C3" t="str">
+        <v>35</v>
+      </c>
+      <c r="D3" t="str">
+        <v>50</v>
+      </c>
+      <c r="E3" t="str">
+        <v>Maivelyn</v>
+      </c>
+      <c r="F3" t="str">
+        <v>maivelynn@gmail.com</v>
+      </c>
+      <c r="G3" t="str">
+        <v>92929292</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
-      <c r="I3" t="s">
-        <v>5</v>
+      <c r="I3" t="str">
+        <v>2026-01-11T14:33:36.988Z</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4">
-        <v>56936300432</v>
-      </c>
-      <c r="E4">
-        <v>10</v>
-      </c>
-      <c r="F4">
-        <v>30</v>
-      </c>
-      <c r="G4">
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Confección - Blusas</v>
+      </c>
+      <c r="B4">
         <v>1</v>
+      </c>
+      <c r="C4" t="str">
+        <v>45</v>
+      </c>
+      <c r="D4" t="str">
+        <v>60</v>
+      </c>
+      <c r="E4" t="str">
+        <v>Maivelyn</v>
+      </c>
+      <c r="F4" t="str">
+        <v>maivelynn@gmail.com</v>
+      </c>
+      <c r="G4" t="str">
+        <v>92929292</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
-      <c r="I4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5">
-        <v>56992914526</v>
-      </c>
-      <c r="E5">
-        <v>42</v>
-      </c>
-      <c r="F5">
-        <v>50</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5" t="s">
-        <v>5</v>
+      <c r="I4" t="str">
+        <v>2026-01-11T14:34:03.795Z</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="B1:C1 B4:C4 G2 D1 G1 C5 D4:D5 G5 G3 G4:I4 I2 I3 I5 I1" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>